<commit_message>
Updated BGR model - 2025-08-06 00:19
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_BGR/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E17FC5-938C-4FA2-A342-6164E141AD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32B5AD0-C755-43B9-B08F-6EB2852666D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S2b0322h12,S3aH3,S5c1016h09,S4aH2,S5d1127h07,S4aH5,S5d1127h08,S5d1127h14,S3aH5,S5aH3,S5d1127h16,S5d1127h18,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5c1016h12,S5c1016h13,S6aH2,S2b0322h11,S5c1016h07,S5c1016h11,S5c1016h15,S1aH2,S2aH3,S2b0322h18,S2b0322h09,S5c1016h08,S5c1016h16,S5d1127h12,S2b0322h07,S2b0322h17,S5c1016h17,S5d1127h10,S6aH5,S3aH4,S4aH3,S4aH4,S5c1016h14,S2b0322h08,S2b0322h15,S2b0322h16,S5c1016h18,S5d1127h17,S1aH3,S5c1016h10,S2b0322h10,S2b0322h13,S2b0322h14,S5aH4,S5d1127h09,S5d1127h11,S5d1127h13,S5d1127h15,S6aH3,S6aH4,S1aH4,S2aH2,S3aH2</t>
-  </si>
-  <si>
-    <t>S2b0322h01,S5c1016h06,S5d1127h23,S6aH8,S2b0322h05,S2b0322h22,S2b0322h23,S4aH6,S5d1127h20,S5d1127h24,S2aH1,S3aH7,S5aH8,S5c1016h21,S5d1127h03,S5d1127h04,S1aH8,S2b0322h20,S5aH1,S5c1016h24,S6aH7,S1aH6,S2b0322h19,S5c1016h05,S2aH6,S3aH1,S5c1016h20,S5d1127h19,S2b0322h02,S2b0322h21,S5d1127h02,S2aH8,S2b0322h24,S5c1016h02,S5c1016h04,S5c1016h22,S5d1127h05,S5d1127h06,S5d1127h21,S5d1127h22,S4aH8,S5c1016h01,S5c1016h19,S5d1127h01,S5c1016h23,S1aH1,S2aH7,S1aH7,S2b0322h03,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S2b0322h06,S5c1016h03,S4aH1,S6aH1,S2b0322h04,S3aH8</t>
+    <t>S2b0322h09,S5c1016h08,S5c1016h16,S5d1127h12,S3aH5,S5aH3,S5d1127h16,S5d1127h18,S1aH4,S2aH2,S2b0322h10,S2b0322h13,S2b0322h14,S5aH4,S5d1127h09,S5d1127h11,S5d1127h13,S5d1127h15,S6aH3,S6aH4,S1aH2,S2aH3,S2b0322h18,S2b0322h08,S2b0322h15,S2b0322h16,S5c1016h18,S5d1127h17,S1aH3,S5c1016h10,S2b0322h12,S2b0322h11,S5c1016h07,S5c1016h11,S5c1016h15,S2b0322h07,S2b0322h17,S5c1016h17,S5d1127h10,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5c1016h12,S5c1016h13,S6aH2,S3aH4,S4aH3,S4aH4,S5c1016h14,S3aH3,S5c1016h09,S3aH2,S4aH2,S5d1127h07,S4aH5,S5d1127h08,S5d1127h14</t>
+  </si>
+  <si>
+    <t>S2aH8,S2b0322h24,S5c1016h02,S5c1016h04,S5c1016h22,S5d1127h05,S5d1127h06,S5d1127h21,S5d1127h22,S1aH8,S2b0322h20,S5aH1,S5c1016h24,S6aH7,S4aH1,S6aH1,S2b0322h06,S5c1016h03,S2b0322h02,S2b0322h21,S5d1127h02,S1aH1,S2aH7,S1aH7,S2b0322h03,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S2b0322h01,S5c1016h06,S5d1127h23,S6aH8,S2aH6,S3aH1,S5c1016h20,S5d1127h19,S4aH8,S5c1016h01,S5c1016h19,S5d1127h01,S1aH6,S2b0322h19,S5c1016h05,S5c1016h23,S2b0322h05,S2b0322h22,S2b0322h23,S4aH6,S5d1127h20,S5d1127h24,S2b0322h04,S3aH8,S2aH1,S3aH7,S5aH8,S5c1016h21,S5d1127h03,S5d1127h04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2b0322h01,S5c1016h06,S5d1127h23,S6aH8,S2b0322h05,S2b0322h22,S2b0322h23,S4aH6,S5d1127h20,S5d1127h24,S2aH1,S3aH7,S5aH8,S5c1016h21,S5d1127h03,S5d1127h04,S1aH8,S2b0322h20,S5aH1,S5c1016h24,S6aH7,S1aH6,S2b0322h19,S5c1016h05,S2aH6,S3aH1,S5c1016h20,S5d1127h19,S2b0322h02,S2b0322h21,S5d1127h02,S2aH8,S2b0322h24,S5c1016h02,S5c1016h04,S5c1016h22,S5d1127h05,S5d1127h06,S5d1127h21,S5d1127h22,S4aH8,S5c1016h01,S5c1016h19,S5d1127h01,S5c1016h23,S1aH1,S2aH7,S1aH7,S2b0322h03,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S2b0322h06,S5c1016h03,S4aH1,S6aH1,S2b0322h04,S3aH8</v>
+        <v>S2aH8,S2b0322h24,S5c1016h02,S5c1016h04,S5c1016h22,S5d1127h05,S5d1127h06,S5d1127h21,S5d1127h22,S1aH8,S2b0322h20,S5aH1,S5c1016h24,S6aH7,S4aH1,S6aH1,S2b0322h06,S5c1016h03,S2b0322h02,S2b0322h21,S5d1127h02,S1aH1,S2aH7,S1aH7,S2b0322h03,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S2b0322h01,S5c1016h06,S5d1127h23,S6aH8,S2aH6,S3aH1,S5c1016h20,S5d1127h19,S4aH8,S5c1016h01,S5c1016h19,S5d1127h01,S1aH6,S2b0322h19,S5c1016h05,S5c1016h23,S2b0322h05,S2b0322h22,S2b0322h23,S4aH6,S5d1127h20,S5d1127h24,S2b0322h04,S3aH8,S2aH1,S3aH7,S5aH8,S5c1016h21,S5d1127h03,S5d1127h04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S2b0322h12,S3aH3,S5c1016h09,S4aH2,S5d1127h07,S4aH5,S5d1127h08,S5d1127h14,S3aH5,S5aH3,S5d1127h16,S5d1127h18,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5c1016h12,S5c1016h13,S6aH2,S2b0322h11,S5c1016h07,S5c1016h11,S5c1016h15,S1aH2,S2aH3,S2b0322h18,S2b0322h09,S5c1016h08,S5c1016h16,S5d1127h12,S2b0322h07,S2b0322h17,S5c1016h17,S5d1127h10,S6aH5,S3aH4,S4aH3,S4aH4,S5c1016h14,S2b0322h08,S2b0322h15,S2b0322h16,S5c1016h18,S5d1127h17,S1aH3,S5c1016h10,S2b0322h10,S2b0322h13,S2b0322h14,S5aH4,S5d1127h09,S5d1127h11,S5d1127h13,S5d1127h15,S6aH3,S6aH4,S1aH4,S2aH2,S3aH2</v>
+        <v>S2b0322h09,S5c1016h08,S5c1016h16,S5d1127h12,S3aH5,S5aH3,S5d1127h16,S5d1127h18,S1aH4,S2aH2,S2b0322h10,S2b0322h13,S2b0322h14,S5aH4,S5d1127h09,S5d1127h11,S5d1127h13,S5d1127h15,S6aH3,S6aH4,S1aH2,S2aH3,S2b0322h18,S2b0322h08,S2b0322h15,S2b0322h16,S5c1016h18,S5d1127h17,S1aH3,S5c1016h10,S2b0322h12,S2b0322h11,S5c1016h07,S5c1016h11,S5c1016h15,S2b0322h07,S2b0322h17,S5c1016h17,S5d1127h10,S6aH5,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S5c1016h12,S5c1016h13,S6aH2,S3aH4,S4aH3,S4aH4,S5c1016h14,S3aH3,S5c1016h09,S3aH2,S4aH2,S5d1127h07,S4aH5,S5d1127h08,S5d1127h14</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC262A7E-512D-4F32-A78F-DEAF1BA2C7EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73AB4099-189F-4DA5-B35F-5DC5E2E918FC}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7682698F-D72E-405E-9B10-1D7B9CD6166C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083344B2-9BE3-4AF3-ABC3-DDF0F6D9D833}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,10 +2945,10 @@
         <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="N4">
-        <v>0.19076754984976782</v>
+        <v>8.161704452335429E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="N5">
-        <v>0.12029500136574706</v>
+        <v>0.52706910680142027</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N6">
-        <v>8.161704452335429E-2</v>
+        <v>0.12029500136574706</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N7">
-        <v>0.52706910680142027</v>
+        <v>0.1465173449877083</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>0.1465173449877083</v>
+        <v>0.19076754984976782</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D31F80-7B40-44DF-A4A6-C7FF052A6494}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6CDBBA-827E-442D-A333-11454DB6A7EB}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>